<commit_message>
Added funtionalities like error handling and authentication to main.py
</commit_message>
<xml_diff>
--- a/output/houses.xlsx
+++ b/output/houses.xlsx
@@ -1011,10 +1011,10 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>240000</v>
+        <v>155000</v>
       </c>
       <c r="B25" t="n">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C25" t="n">
         <v>2</v>
@@ -1024,117 +1024,117 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Santa Justa - Miraflores - Cruz Roja</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Luis Montoto - Santa Justa</t>
+          <t>Arroyo - Santa Justa</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>239900</v>
+        <v>205000</v>
       </c>
       <c r="B26" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>La Palmera - Los Bermejales</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Luis Montoto - Santa Justa</t>
+          <t>Bami - Pineda</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>155000</v>
+        <v>280000</v>
       </c>
       <c r="B27" t="n">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Santa Justa - Miraflores - Cruz Roja</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Arroyo - Santa Justa</t>
+          <t>Arenal - Museo - Tetuán</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>205000</v>
+        <v>230000</v>
       </c>
       <c r="B28" t="n">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
         <v>2</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>La Palmera - Los Bermejales</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Bami - Pineda</t>
+          <t>López de Gomara</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>280000</v>
+        <v>320000</v>
       </c>
       <c r="B29" t="n">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C29" t="n">
         <v>3</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Arenal - Museo - Tetuán</t>
+          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>320000</v>
+        <v>280000</v>
       </c>
       <c r="B30" t="n">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C30" t="n">
         <v>3</v>
@@ -1144,45 +1144,45 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
+          <t>Gran Plaza - Marqués de Pickman - Ciudad Jardín</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>230000</v>
+        <v>359000</v>
       </c>
       <c r="B31" t="n">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
         <v>2</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>López de Gomara</t>
+          <t>Nervión</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>550000</v>
+        <v>339000</v>
       </c>
       <c r="B32" t="n">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C32" t="n">
         <v>3</v>
@@ -1192,21 +1192,21 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Arenal - Museo - Tetuán</t>
+          <t>Calle Betis - Pagés del Corro</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>359000</v>
+        <v>550000</v>
       </c>
       <c r="B33" t="n">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="C33" t="n">
         <v>3</v>
@@ -1216,27 +1216,27 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Arenal - Museo - Tetuán</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>280000</v>
+        <v>789000</v>
       </c>
       <c r="B34" t="n">
-        <v>80</v>
+        <v>286</v>
       </c>
       <c r="C34" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1245,88 +1245,88 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Gran Plaza - Marqués de Pickman - Ciudad Jardín</t>
+          <t>Buhaira - Huerta del Rey</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>339000</v>
+        <v>170000</v>
       </c>
       <c r="B35" t="n">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="C35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>Santa Justa - Miraflores - Cruz Roja</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Calle Betis - Pagés del Corro</t>
+          <t>Arroyo - Santa Justa</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>789000</v>
+        <v>330000</v>
       </c>
       <c r="B36" t="n">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="C36" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D36" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Los Remedios</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Buhaira - Huerta del Rey</t>
+          <t>Ramón de Carranza - Madre Rafols</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>330000</v>
+        <v>250000</v>
       </c>
       <c r="B37" t="n">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C37" t="n">
         <v>3</v>
       </c>
       <c r="D37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Los Remedios</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Ramón de Carranza - Madre Rafols</t>
+          <t>Puerta Carmona-Puerta Osario-Amador de los Ríos</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>170000</v>
+        <v>300000</v>
       </c>
       <c r="B38" t="n">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="C38" t="n">
         <v>2</v>
@@ -1336,12 +1336,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Santa Justa - Miraflores - Cruz Roja</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Arroyo - Santa Justa</t>
+          <t>San Vicente</t>
         </is>
       </c>
     </row>
@@ -1371,64 +1371,64 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>300000</v>
+        <v>499000</v>
       </c>
       <c r="B40" t="n">
-        <v>100</v>
+        <v>189</v>
       </c>
       <c r="C40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Los Remedios</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>San Vicente</t>
+          <t>Ramón de Carranza - Madre Rafols</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>250000</v>
+        <v>349000</v>
       </c>
       <c r="B41" t="n">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="C41" t="n">
         <v>3</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Puerta Carmona-Puerta Osario-Amador de los Ríos</t>
+          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>349000</v>
+        <v>295000</v>
       </c>
       <c r="B42" t="n">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C42" t="n">
         <v>3</v>
       </c>
       <c r="D42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1437,142 +1437,142 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
+          <t>López de Gomara</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>499000</v>
+        <v>380000</v>
       </c>
       <c r="B43" t="n">
         <v>189</v>
       </c>
       <c r="C43" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Los Remedios</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Ramón de Carranza - Madre Rafols</t>
+          <t>Nervión</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>295000</v>
+        <v>330000</v>
       </c>
       <c r="B44" t="n">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="C44" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>López de Gomara</t>
+          <t>Nervión</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>330000</v>
+        <v>372000</v>
       </c>
       <c r="B45" t="n">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>San Vicente</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>380000</v>
+        <v>368000</v>
       </c>
       <c r="B46" t="n">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="C46" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>San Vicente</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>372000</v>
+        <v>290000</v>
       </c>
       <c r="B47" t="n">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="C47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>San Vicente</t>
+          <t>Luis Montoto - Santa Justa</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>368000</v>
+        <v>1495000</v>
       </c>
       <c r="B48" t="n">
-        <v>90</v>
+        <v>346</v>
       </c>
       <c r="C48" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1581,79 +1581,79 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>San Vicente</t>
+          <t>Santa Cruz - Alfalfa</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>290000</v>
+        <v>132260</v>
       </c>
       <c r="B49" t="n">
         <v>114</v>
       </c>
       <c r="C49" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" t="n">
         <v>2</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Cerro Amate</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Luis Montoto - Santa Justa</t>
+          <t>Santa Aurelia</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1495000</v>
+        <v>450000</v>
       </c>
       <c r="B50" t="n">
-        <v>346</v>
+        <v>114</v>
       </c>
       <c r="C50" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Santa Cruz - Alfalfa</t>
+          <t>Nervión</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>132260</v>
+        <v>575000</v>
       </c>
       <c r="B51" t="n">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="C51" t="n">
         <v>4</v>
       </c>
       <c r="D51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Cerro Amate</t>
+          <t>Prado de San Sebastián - Felipe II - Bueno Monreal</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Santa Aurelia</t>
+          <t>Felipe II - Bueno Monreal</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Created SQLite database, modules in package 'app' and minor changes
</commit_message>
<xml_diff>
--- a/output/houses.xlsx
+++ b/output/houses.xlsx
@@ -987,109 +987,109 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1565000</v>
+        <v>789000</v>
       </c>
       <c r="B24" t="n">
-        <v>256</v>
+        <v>286</v>
       </c>
       <c r="C24" t="n">
         <v>6</v>
       </c>
       <c r="D24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Arenal - Museo - Tetuán</t>
+          <t>Buhaira - Huerta del Rey</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>155000</v>
+        <v>1565000</v>
       </c>
       <c r="B25" t="n">
-        <v>66</v>
+        <v>256</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Santa Justa - Miraflores - Cruz Roja</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Arroyo - Santa Justa</t>
+          <t>Arenal - Museo - Tetuán</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>205000</v>
+        <v>230000</v>
       </c>
       <c r="B26" t="n">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
         <v>2</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>La Palmera - Los Bermejales</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Bami - Pineda</t>
+          <t>López de Gomara</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>280000</v>
+        <v>155000</v>
       </c>
       <c r="B27" t="n">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Santa Justa - Miraflores - Cruz Roja</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Arenal - Museo - Tetuán</t>
+          <t>Arroyo - Santa Justa</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>230000</v>
+        <v>320000</v>
       </c>
       <c r="B28" t="n">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
         <v>2</v>
@@ -1101,16 +1101,16 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>López de Gomara</t>
+          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>320000</v>
+        <v>205000</v>
       </c>
       <c r="B29" t="n">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C29" t="n">
         <v>3</v>
@@ -1120,12 +1120,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>La Palmera - Los Bermejales</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
+          <t>Bami - Pineda</t>
         </is>
       </c>
     </row>
@@ -1134,22 +1134,22 @@
         <v>280000</v>
       </c>
       <c r="B30" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C30" t="n">
         <v>3</v>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Gran Plaza - Marqués de Pickman - Ciudad Jardín</t>
+          <t>Arenal - Museo - Tetuán</t>
         </is>
       </c>
     </row>
@@ -1203,10 +1203,10 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>550000</v>
+        <v>280000</v>
       </c>
       <c r="B33" t="n">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="C33" t="n">
         <v>3</v>
@@ -1216,84 +1216,84 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Arenal - Museo - Tetuán</t>
+          <t>Gran Plaza - Marqués de Pickman - Ciudad Jardín</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>789000</v>
+        <v>550000</v>
       </c>
       <c r="B34" t="n">
-        <v>286</v>
+        <v>124</v>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D34" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Buhaira - Huerta del Rey</t>
+          <t>Arenal - Museo - Tetuán</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>170000</v>
+        <v>330000</v>
       </c>
       <c r="B35" t="n">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="C35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Santa Justa - Miraflores - Cruz Roja</t>
+          <t>Los Remedios</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Arroyo - Santa Justa</t>
+          <t>Ramón de Carranza - Madre Rafols</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>330000</v>
+        <v>170000</v>
       </c>
       <c r="B36" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Los Remedios</t>
+          <t>Santa Justa - Miraflores - Cruz Roja</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Ramón de Carranza - Madre Rafols</t>
+          <t>Arroyo - Santa Justa</t>
         </is>
       </c>
     </row>
@@ -1323,97 +1323,97 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>300000</v>
+        <v>289000</v>
       </c>
       <c r="B38" t="n">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>San Vicente</t>
+          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>289000</v>
+        <v>300000</v>
       </c>
       <c r="B39" t="n">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
+          <t>San Vicente</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>499000</v>
+        <v>349000</v>
       </c>
       <c r="B40" t="n">
-        <v>189</v>
+        <v>126</v>
       </c>
       <c r="C40" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40" t="n">
         <v>2</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Los Remedios</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Ramón de Carranza - Madre Rafols</t>
+          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>349000</v>
+        <v>499000</v>
       </c>
       <c r="B41" t="n">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="C41" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D41" t="n">
         <v>2</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>Los Remedios</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Ronda de Triana-Patrocinio-Turruñuelo</t>
+          <t>Ramón de Carranza - Madre Rafols</t>
         </is>
       </c>
     </row>
@@ -1443,40 +1443,40 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>380000</v>
+        <v>368000</v>
       </c>
       <c r="B43" t="n">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="C43" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>San Vicente</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>330000</v>
+        <v>380000</v>
       </c>
       <c r="B44" t="n">
-        <v>140</v>
+        <v>189</v>
       </c>
       <c r="C44" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1491,40 +1491,40 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>372000</v>
+        <v>330000</v>
       </c>
       <c r="B45" t="n">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>San Vicente</t>
+          <t>Nervión</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>368000</v>
+        <v>372000</v>
       </c>
       <c r="B46" t="n">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C46" t="n">
         <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1635,25 +1635,25 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>575000</v>
+        <v>239900</v>
       </c>
       <c r="B51" t="n">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="C51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Prado de San Sebastián - Felipe II - Bueno Monreal</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Felipe II - Bueno Monreal</t>
+          <t>Luis Montoto - Santa Justa</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Created file filters.json so filter parameters are not stored within the main.py
</commit_message>
<xml_diff>
--- a/output/houses.xlsx
+++ b/output/houses.xlsx
@@ -1035,49 +1035,49 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>230000</v>
+        <v>205000</v>
       </c>
       <c r="B26" t="n">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
         <v>2</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>La Palmera - Los Bermejales</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>López de Gomara</t>
+          <t>Bami - Pineda</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>155000</v>
+        <v>230000</v>
       </c>
       <c r="B27" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C27" t="n">
         <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Santa Justa - Miraflores - Cruz Roja</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Arroyo - Santa Justa</t>
+          <t>López de Gomara</t>
         </is>
       </c>
     </row>
@@ -1107,25 +1107,25 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>205000</v>
+        <v>155000</v>
       </c>
       <c r="B29" t="n">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>La Palmera - Los Bermejales</t>
+          <t>Santa Justa - Miraflores - Cruz Roja</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Bami - Pineda</t>
+          <t>Arroyo - Santa Justa</t>
         </is>
       </c>
     </row>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>339000</v>
+        <v>550000</v>
       </c>
       <c r="B32" t="n">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C32" t="n">
         <v>3</v>
@@ -1192,21 +1192,21 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Triana</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Calle Betis - Pagés del Corro</t>
+          <t>Arenal - Museo - Tetuán</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>280000</v>
+        <v>339000</v>
       </c>
       <c r="B33" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C33" t="n">
         <v>3</v>
@@ -1216,21 +1216,21 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Gran Plaza - Marqués de Pickman - Ciudad Jardín</t>
+          <t>Calle Betis - Pagés del Corro</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>550000</v>
+        <v>280000</v>
       </c>
       <c r="B34" t="n">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="C34" t="n">
         <v>3</v>
@@ -1240,60 +1240,60 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Arenal - Museo - Tetuán</t>
+          <t>Gran Plaza - Marqués de Pickman - Ciudad Jardín</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>330000</v>
+        <v>170000</v>
       </c>
       <c r="B35" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Los Remedios</t>
+          <t>Santa Justa - Miraflores - Cruz Roja</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Ramón de Carranza - Madre Rafols</t>
+          <t>Arroyo - Santa Justa</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>170000</v>
+        <v>330000</v>
       </c>
       <c r="B36" t="n">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="C36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Santa Justa - Miraflores - Cruz Roja</t>
+          <t>Los Remedios</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Arroyo - Santa Justa</t>
+          <t>Ramón de Carranza - Madre Rafols</t>
         </is>
       </c>
     </row>
@@ -1443,97 +1443,97 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>368000</v>
+        <v>330000</v>
       </c>
       <c r="B43" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="C43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D43" t="n">
         <v>2</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>San Vicente</t>
+          <t>Nervión</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>380000</v>
+        <v>372000</v>
       </c>
       <c r="B44" t="n">
-        <v>189</v>
+        <v>99</v>
       </c>
       <c r="C44" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>San Vicente</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>330000</v>
+        <v>368000</v>
       </c>
       <c r="B45" t="n">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D45" t="n">
         <v>2</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>San Vicente</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>372000</v>
+        <v>380000</v>
       </c>
       <c r="B46" t="n">
-        <v>99</v>
+        <v>189</v>
       </c>
       <c r="C46" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Nervión</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>San Vicente</t>
+          <t>Nervión</t>
         </is>
       </c>
     </row>
@@ -1563,49 +1563,49 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1495000</v>
+        <v>132260</v>
       </c>
       <c r="B48" t="n">
-        <v>346</v>
+        <v>114</v>
       </c>
       <c r="C48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Centro</t>
+          <t>Cerro Amate</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Santa Cruz - Alfalfa</t>
+          <t>Santa Aurelia</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>132260</v>
+        <v>1495000</v>
       </c>
       <c r="B49" t="n">
-        <v>114</v>
+        <v>346</v>
       </c>
       <c r="C49" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Cerro Amate</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Santa Aurelia</t>
+          <t>Santa Cruz - Alfalfa</t>
         </is>
       </c>
     </row>
@@ -1635,25 +1635,25 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>239900</v>
+        <v>425000</v>
       </c>
       <c r="B51" t="n">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="C51" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Nervión</t>
+          <t>Triana</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Luis Montoto - Santa Justa</t>
+          <t>López de Gomara</t>
         </is>
       </c>
     </row>

</xml_diff>